<commit_message>
updated schematic component designations.
</commit_message>
<xml_diff>
--- a/Car_Circuitry/Car_Circuitry_BOM.xlsx
+++ b/Car_Circuitry/Car_Circuitry_BOM.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Oasis\Documents\School\Assignments\Undergraduate Year 3\Chem-E Car Team\Car_Circuitry\Project Outputs for Car_Circuitry\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Oasis\Documents\School\Assignments\Undergraduate Year 3\Chem-E Car Team\McMaster_Chem-E_Car_23-24\Car_Circuitry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CA6F5225-EFA8-49AE-8419-B4EFDCD7B27F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E715B02-9158-48E9-A839-9FE99FBD537C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="760" windowWidth="16800" windowHeight="9760" xr2:uid="{9CFF55D9-0FD4-4840-8105-D7C1343FE60D}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13620" xr2:uid="{88E1D610-4988-495D-931A-50350FD2D97D}"/>
   </bookViews>
   <sheets>
-    <sheet name="Car_Circuitry" sheetId="1" r:id="rId1"/>
+    <sheet name="Car_Circuitry_BOM" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">Car_Circuitry!$1:$1</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">Car_Circuitry_BOM!$1:$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="111">
   <si>
     <t>Comment</t>
   </si>
@@ -59,165 +59,192 @@
     <t>Quantity</t>
   </si>
   <si>
+    <t>2601-3102</t>
+  </si>
+  <si>
+    <t>WAGO Terminal Block</t>
+  </si>
+  <si>
+    <t>BAT_IN</t>
+  </si>
+  <si>
+    <t>26013102</t>
+  </si>
+  <si>
+    <t>MP3213DH-LF-P</t>
+  </si>
+  <si>
+    <t>Integrated Circuit</t>
+  </si>
+  <si>
+    <t>BOOST1</t>
+  </si>
+  <si>
+    <t>SOP65P490X110-9N</t>
+  </si>
+  <si>
+    <t>TPS61023DRLT</t>
+  </si>
+  <si>
+    <t>BOOST2</t>
+  </si>
+  <si>
+    <t>SOTFL50P160X60-6N</t>
+  </si>
+  <si>
+    <t>2.2 nF</t>
+  </si>
+  <si>
+    <t>Capacitor</t>
+  </si>
+  <si>
+    <t>C1, C12</t>
+  </si>
+  <si>
+    <t>CAPC2012X75N</t>
+  </si>
+  <si>
+    <t>CL21B222KBANNNC</t>
+  </si>
+  <si>
+    <t>10 nF</t>
+  </si>
+  <si>
+    <t>C2, C5, C6, C17</t>
+  </si>
+  <si>
+    <t>CL21B103KBANNNC</t>
+  </si>
+  <si>
+    <t>10 μF</t>
+  </si>
+  <si>
+    <t>C3, C7, C8, C14</t>
+  </si>
+  <si>
+    <t>CAPC2012X140N</t>
+  </si>
+  <si>
+    <t>CL21B106KOQNNNE</t>
+  </si>
+  <si>
+    <t>4.7 μF</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>CAPC2012X135N</t>
+  </si>
+  <si>
+    <t>CL21B475KOFNNNE</t>
+  </si>
+  <si>
+    <t>2.2 μF</t>
+  </si>
+  <si>
+    <t>C9, C10</t>
+  </si>
+  <si>
+    <t>CL21B225KAFNNWE</t>
+  </si>
+  <si>
+    <t>100 nF</t>
+  </si>
+  <si>
+    <t>C11, C13</t>
+  </si>
+  <si>
+    <t>CAPC2012X95N</t>
+  </si>
+  <si>
+    <t>CL21B104KBCNNNC</t>
+  </si>
+  <si>
+    <t>22 μF</t>
+  </si>
+  <si>
+    <t>C15, C16</t>
+  </si>
+  <si>
+    <t>CAPC3216X180N</t>
+  </si>
+  <si>
+    <t>CL31B226KPHNNNE</t>
+  </si>
+  <si>
+    <t>CUHS20S30,H3F</t>
+  </si>
+  <si>
+    <t>Schottky Diode</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>CUHS20S40H3F</t>
+  </si>
+  <si>
+    <t>DRV8833PWPR</t>
+  </si>
+  <si>
+    <t>DRV1, DRV2</t>
+  </si>
+  <si>
+    <t>SOP65P640X120-17N</t>
+  </si>
+  <si>
+    <t>DRV8833PWP</t>
+  </si>
+  <si>
+    <t>B3B-XH-A(LF)(SN)</t>
+  </si>
+  <si>
+    <t>CONN HEADER VERT 3POS 2.5MM</t>
+  </si>
+  <si>
+    <t>DS18B20_IN, SER0039_OUT</t>
+  </si>
+  <si>
+    <t>FP-B3B-XH-A_LF_SN-MFG</t>
+  </si>
+  <si>
+    <t>CMP-17439-000014-3</t>
+  </si>
+  <si>
     <t>MPU6050</t>
   </si>
   <si>
-    <t>Integrated Circuit</t>
-  </si>
-  <si>
-    <t>ACCEL</t>
-  </si>
-  <si>
-    <t>2601-3102</t>
-  </si>
-  <si>
-    <t>Connector</t>
-  </si>
-  <si>
-    <t>BAT_IN</t>
-  </si>
-  <si>
-    <t>26013102</t>
-  </si>
-  <si>
-    <t>MP3213DH-LF-P</t>
-  </si>
-  <si>
-    <t>BOOST1</t>
-  </si>
-  <si>
-    <t>SOP65P490X110-9N</t>
-  </si>
-  <si>
-    <t>TPS61023DRLT</t>
-  </si>
-  <si>
-    <t>BOOST2</t>
-  </si>
-  <si>
-    <t>SOTFL50P160X60-6N</t>
-  </si>
-  <si>
-    <t>CL21B222KBANNNC</t>
-  </si>
-  <si>
-    <t>Capacitor</t>
-  </si>
-  <si>
-    <t>C1, C12</t>
-  </si>
-  <si>
-    <t>CAPC2012X75N</t>
-  </si>
-  <si>
-    <t>CL21B103KBANNNC</t>
-  </si>
-  <si>
-    <t>C2, C5, C6, C17</t>
-  </si>
-  <si>
-    <t>CL21B106KOQNNNE</t>
-  </si>
-  <si>
-    <t>C3, C7, C8, C14</t>
-  </si>
-  <si>
-    <t>CAPC2012X140N</t>
-  </si>
-  <si>
-    <t>CL21B475KOFNNNE</t>
-  </si>
-  <si>
-    <t>C4</t>
-  </si>
-  <si>
-    <t>CAPC2012X135N</t>
-  </si>
-  <si>
-    <t>CL21B225KAFNNWE</t>
-  </si>
-  <si>
-    <t>C9, C10</t>
-  </si>
-  <si>
-    <t>CL21B104KBCNNNC</t>
-  </si>
-  <si>
-    <t>C11, C13</t>
-  </si>
-  <si>
-    <t>CAPC2012X95N</t>
-  </si>
-  <si>
-    <t>CL31B226KPHNNNE</t>
-  </si>
-  <si>
-    <t>C15, C16</t>
-  </si>
-  <si>
-    <t>CAPC3216X180N</t>
-  </si>
-  <si>
-    <t>CUHS20S30,H3F</t>
-  </si>
-  <si>
-    <t>Schottky Diode</t>
-  </si>
-  <si>
-    <t>D1</t>
-  </si>
-  <si>
-    <t>CUHS20S40H3F</t>
-  </si>
-  <si>
-    <t>DRV8833PWPR</t>
-  </si>
-  <si>
-    <t>DRV1, DRV2</t>
-  </si>
-  <si>
-    <t>SOP65P640X120-17N</t>
-  </si>
-  <si>
-    <t>DRV8833PWP</t>
-  </si>
-  <si>
-    <t>B3B-XH-A(LF)(SN)</t>
-  </si>
-  <si>
-    <t>CONN HEADER VERT 3POS 2.5MM</t>
-  </si>
-  <si>
-    <t>DS18B20_IN, SER0039_OUT</t>
-  </si>
-  <si>
-    <t>FP-B3B-XH-A_LF_SN-MFG</t>
-  </si>
-  <si>
-    <t>CMP-17439-000014-3</t>
+    <t>IMU</t>
+  </si>
+  <si>
+    <t>4.7 μH</t>
+  </si>
+  <si>
+    <t>Inductor</t>
+  </si>
+  <si>
+    <t>L1</t>
+  </si>
+  <si>
+    <t>DFE2HCAH1R0MJ0L</t>
   </si>
   <si>
     <t>DFE252012P-4R7M=P2</t>
   </si>
   <si>
-    <t>Inductor</t>
-  </si>
-  <si>
-    <t>L1</t>
-  </si>
-  <si>
-    <t>DFE2HCAH1R0MJ0L</t>
+    <t>1 μH</t>
+  </si>
+  <si>
+    <t>L2</t>
+  </si>
+  <si>
+    <t>1286ASH1R0MP2</t>
   </si>
   <si>
     <t>DFE201612E-1R0M=P2</t>
   </si>
   <si>
-    <t>L2</t>
-  </si>
-  <si>
-    <t>1286ASH1R0MP2</t>
-  </si>
-  <si>
     <t>B2B-XH-A(LF)(SN)</t>
   </si>
   <si>
@@ -233,91 +260,124 @@
     <t>CMP-2000-05888-3</t>
   </si>
   <si>
+    <t>Feather M0 Adalogger</t>
+  </si>
+  <si>
+    <t>Adafruit Microcontroller</t>
+  </si>
+  <si>
+    <t>MCU</t>
+  </si>
+  <si>
     <t>2796</t>
   </si>
   <si>
-    <t>MCU</t>
+    <t>15 kΩ</t>
+  </si>
+  <si>
+    <t>Resistor</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>RESC3216X70N</t>
   </si>
   <si>
     <t>RMCF1206FT15K0</t>
   </si>
   <si>
-    <t>Resistor</t>
-  </si>
-  <si>
-    <t>R1</t>
-  </si>
-  <si>
-    <t>RESC3216X70N</t>
+    <t>10 kΩ</t>
+  </si>
+  <si>
+    <t>R2</t>
   </si>
   <si>
     <t>RMCF1206FT10K0</t>
   </si>
   <si>
-    <t>R2</t>
+    <t>75 kΩ</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>RESC3116X65N</t>
   </si>
   <si>
     <t>RC1206FR-0775KL</t>
   </si>
   <si>
-    <t>R3</t>
-  </si>
-  <si>
-    <t>RESC3116X65N</t>
+    <t>2.2 kΩ</t>
+  </si>
+  <si>
+    <t>R4, R7</t>
+  </si>
+  <si>
+    <t>RESAD1042W49L330D178</t>
   </si>
   <si>
     <t>RNMF14FTC2K20</t>
   </si>
   <si>
-    <t>R4, R7</t>
-  </si>
-  <si>
-    <t>RESAD1042W49L330D178</t>
+    <t>180 mΩ</t>
+  </si>
+  <si>
+    <t>R5, R8</t>
+  </si>
+  <si>
+    <t>ERJ6_B_BW_R_LW_CW_D</t>
   </si>
   <si>
     <t>ERJ-6DSFR18V</t>
   </si>
   <si>
-    <t>R5, R8</t>
-  </si>
-  <si>
-    <t>ERJ6_B_BW_R_LW_CW_D</t>
+    <t>330 mΩ</t>
+  </si>
+  <si>
+    <t>R6, R9</t>
   </si>
   <si>
     <t>ERJ-6DQFR33V</t>
   </si>
   <si>
-    <t>R6, R9</t>
+    <t>4.7 kΩ</t>
+  </si>
+  <si>
+    <t>R10</t>
+  </si>
+  <si>
+    <t>RESAD1530W60L610D230</t>
   </si>
   <si>
     <t>CF1_4C472J</t>
   </si>
   <si>
-    <t>R10</t>
-  </si>
-  <si>
-    <t>RESAD1530W60L610D230</t>
+    <t>100 kΩ</t>
+  </si>
+  <si>
+    <t>R11</t>
+  </si>
+  <si>
+    <t>ERJ8ENF1000V</t>
   </si>
   <si>
     <t>ERJ-8ENF1003V</t>
   </si>
   <si>
-    <t>R11</t>
-  </si>
-  <si>
-    <t>ERJ8ENF1000V</t>
+    <t>732 kΩ</t>
+  </si>
+  <si>
+    <t>R12</t>
   </si>
   <si>
     <t>ERJ-8ENF7323V</t>
-  </si>
-  <si>
-    <t>R12</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -379,7 +439,9 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{4DB978FA-0150-48E8-B356-EA549AA827AA}"/>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -687,14 +749,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A033821A-F081-4BE3-A85F-D4CCCAD437BB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E0A2440-1AFB-485F-A40A-BAFDD2A1F509}">
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="6" width="18.81640625" customWidth="1"/>
+    <col min="1" max="1" width="19.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.6328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.35">
@@ -728,7 +795,7 @@
         <v>8</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>6</v>
@@ -739,19 +806,19 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>9</v>
       </c>
       <c r="F3" s="1">
         <v>1</v>
@@ -759,19 +826,19 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="F4" s="1">
         <v>1</v>
@@ -779,59 +846,59 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F5" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="E6" s="2" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="F6" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="F7" s="1">
         <v>4</v>
@@ -839,59 +906,59 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="F8" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="F9" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="F10" s="1">
         <v>2</v>
@@ -899,19 +966,19 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="F11" s="1">
         <v>2</v>
@@ -919,59 +986,59 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="F12" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="F13" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>7</v>
+        <v>53</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="F14" s="1">
         <v>2</v>
@@ -979,39 +1046,39 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="F15" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="F16" s="1">
         <v>1</v>
@@ -1019,19 +1086,19 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="F17" s="1">
         <v>1</v>
@@ -1039,19 +1106,19 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="F18" s="1">
         <v>5</v>
@@ -1059,19 +1126,19 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>7</v>
+        <v>74</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="F19" s="1">
         <v>1</v>
@@ -1079,19 +1146,19 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>66</v>
+        <v>81</v>
       </c>
       <c r="F20" s="1">
         <v>1</v>
@@ -1099,19 +1166,19 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>71</v>
+        <v>83</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="F21" s="1">
         <v>1</v>
@@ -1119,19 +1186,19 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="F22" s="1">
         <v>1</v>
@@ -1139,19 +1206,19 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>76</v>
+        <v>90</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>75</v>
+        <v>92</v>
       </c>
       <c r="F23" s="1">
         <v>2</v>
@@ -1159,19 +1226,19 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="C24" s="2" t="s">
-        <v>79</v>
+        <v>94</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>78</v>
+        <v>96</v>
       </c>
       <c r="F24" s="1">
         <v>2</v>
@@ -1179,19 +1246,19 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
-        <v>81</v>
+        <v>97</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>82</v>
+        <v>98</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>81</v>
+        <v>99</v>
       </c>
       <c r="F25" s="1">
         <v>2</v>
@@ -1199,19 +1266,19 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
-        <v>83</v>
+        <v>100</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>84</v>
+        <v>101</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>85</v>
+        <v>102</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="F26" s="1">
         <v>1</v>
@@ -1219,19 +1286,19 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
-        <v>86</v>
+        <v>104</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>87</v>
+        <v>105</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>88</v>
+        <v>106</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>86</v>
+        <v>107</v>
       </c>
       <c r="F27" s="1">
         <v>1</v>
@@ -1239,19 +1306,19 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
-        <v>89</v>
+        <v>108</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>90</v>
+        <v>109</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>88</v>
+        <v>106</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>89</v>
+        <v>110</v>
       </c>
       <c r="F28" s="1">
         <v>1</v>

</xml_diff>

<commit_message>
Changed inductors & boost converter layouts.
</commit_message>
<xml_diff>
--- a/Car_Circuitry/Car_Circuitry_BOM.xlsx
+++ b/Car_Circuitry/Car_Circuitry_BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Oasis\Documents\School\Assignments\Undergraduate Year 3\Chem-E Car Team\McMaster_Chem-E_Car_23-24\Car_Circuitry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E715B02-9158-48E9-A839-9FE99FBD537C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1F7BED0E-A3B2-4EA7-AF96-26B14E2C3F1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13620" xr2:uid="{88E1D610-4988-495D-931A-50350FD2D97D}"/>
+    <workbookView xWindow="0" yWindow="2260" windowWidth="16800" windowHeight="9760" xr2:uid="{056DCDFA-1B32-485B-BDAA-3B4AE06BA512}"/>
   </bookViews>
   <sheets>
     <sheet name="Car_Circuitry_BOM" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="110">
   <si>
     <t>Comment</t>
   </si>
@@ -173,16 +173,16 @@
     <t>CL31B226KPHNNNE</t>
   </si>
   <si>
-    <t>CUHS20S30,H3F</t>
-  </si>
-  <si>
-    <t>Schottky Diode</t>
+    <t>MBRA340T3G</t>
+  </si>
+  <si>
+    <t>Diode</t>
   </si>
   <si>
     <t>D1</t>
   </si>
   <si>
-    <t>CUHS20S40H3F</t>
+    <t>DIOM5226X220N</t>
   </si>
   <si>
     <t>DRV8833PWPR</t>
@@ -227,10 +227,10 @@
     <t>L1</t>
   </si>
   <si>
-    <t>DFE2HCAH1R0MJ0L</t>
-  </si>
-  <si>
-    <t>DFE252012P-4R7M=P2</t>
+    <t>CDRH8D43NP4R7NC</t>
+  </si>
+  <si>
+    <t>CDRH8D43NP-4R7NC</t>
   </si>
   <si>
     <t>1 μH</t>
@@ -239,10 +239,7 @@
     <t>L2</t>
   </si>
   <si>
-    <t>1286ASH1R0MP2</t>
-  </si>
-  <si>
-    <t>DFE201612E-1R0M=P2</t>
+    <t>74438357010</t>
   </si>
   <si>
     <t>B2B-XH-A(LF)(SN)</t>
@@ -377,7 +374,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -439,9 +436,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{4DB978FA-0150-48E8-B356-EA549AA827AA}"/>
-  </tableStyles>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -749,19 +744,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E0A2440-1AFB-485F-A40A-BAFDD2A1F509}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB8CE123-5274-46D9-BAA8-2BCC1D5A76C3}">
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.6328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="6" width="18.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.35">
@@ -1098,7 +1088,7 @@
         <v>66</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F17" s="1">
         <v>1</v>
@@ -1106,19 +1096,19 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="C18" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="D18" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="E18" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>72</v>
       </c>
       <c r="F18" s="1">
         <v>5</v>
@@ -1126,19 +1116,19 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="C19" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="D19" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>76</v>
-      </c>
       <c r="E19" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F19" s="1">
         <v>1</v>
@@ -1146,19 +1136,19 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="C20" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="D20" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="E20" s="2" t="s">
         <v>80</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>81</v>
       </c>
       <c r="F20" s="1">
         <v>1</v>
@@ -1166,19 +1156,19 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C21" s="2" t="s">
+      <c r="D21" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E21" s="2" t="s">
         <v>83</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>84</v>
       </c>
       <c r="F21" s="1">
         <v>1</v>
@@ -1186,19 +1176,19 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C22" s="2" t="s">
+      <c r="D22" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="E22" s="2" t="s">
         <v>87</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>88</v>
       </c>
       <c r="F22" s="1">
         <v>1</v>
@@ -1206,19 +1196,19 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C23" s="2" t="s">
+      <c r="D23" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="E23" s="2" t="s">
         <v>91</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>92</v>
       </c>
       <c r="F23" s="1">
         <v>2</v>
@@ -1226,19 +1216,19 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C24" s="2" t="s">
+      <c r="D24" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="E24" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>96</v>
       </c>
       <c r="F24" s="1">
         <v>2</v>
@@ -1246,19 +1236,19 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B25" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C25" s="2" t="s">
+      <c r="D25" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E25" s="2" t="s">
         <v>98</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>99</v>
       </c>
       <c r="F25" s="1">
         <v>2</v>
@@ -1266,19 +1256,19 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C26" s="2" t="s">
+      <c r="D26" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="E26" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>103</v>
       </c>
       <c r="F26" s="1">
         <v>1</v>
@@ -1286,19 +1276,19 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C27" s="2" t="s">
+      <c r="D27" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="E27" s="2" t="s">
         <v>106</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>107</v>
       </c>
       <c r="F27" s="1">
         <v>1</v>
@@ -1306,19 +1296,19 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C28" s="2" t="s">
+      <c r="D28" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E28" s="2" t="s">
         <v>109</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>110</v>
       </c>
       <c r="F28" s="1">
         <v>1</v>

</xml_diff>

<commit_message>
Final changes to PCB.
</commit_message>
<xml_diff>
--- a/Car_Circuitry/Car_Circuitry_BOM.xlsx
+++ b/Car_Circuitry/Car_Circuitry_BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Oasis\Documents\School\Assignments\Undergraduate Year 3\Chem-E Car Team\McMaster_Chem-E_Car_23-24\Car_Circuitry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1F7BED0E-A3B2-4EA7-AF96-26B14E2C3F1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCDCF3A5-2EA7-40CC-947E-838975E6DD43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2260" windowWidth="16800" windowHeight="9760" xr2:uid="{056DCDFA-1B32-485B-BDAA-3B4AE06BA512}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13620" xr2:uid="{056DCDFA-1B32-485B-BDAA-3B4AE06BA512}"/>
   </bookViews>
   <sheets>
     <sheet name="Car_Circuitry_BOM" sheetId="1" r:id="rId1"/>
@@ -374,7 +374,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -436,7 +436,9 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{6CCABC8B-7800-4CA1-9D47-B37511B91CFF}"/>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -747,11 +749,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB8CE123-5274-46D9-BAA8-2BCC1D5A76C3}">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="6" width="18.81640625" customWidth="1"/>
+    <col min="1" max="1" width="19.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Updated pin assignments & diode part # (backorder)
</commit_message>
<xml_diff>
--- a/Car_Circuitry/Car_Circuitry_BOM.xlsx
+++ b/Car_Circuitry/Car_Circuitry_BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Oasis\Documents\School\Assignments\Undergraduate Year 3\Chem-E Car Team\McMaster_Chem-E_Car_23-24\Car_Circuitry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCDCF3A5-2EA7-40CC-947E-838975E6DD43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B370160B-C190-453C-9D6C-E00CA3122208}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13620" xr2:uid="{056DCDFA-1B32-485B-BDAA-3B4AE06BA512}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13620" xr2:uid="{BFB9A709-E0C0-42D2-9C81-D0328AE637B6}"/>
   </bookViews>
   <sheets>
     <sheet name="Car_Circuitry_BOM" sheetId="1" r:id="rId1"/>
@@ -173,16 +173,16 @@
     <t>CL31B226KPHNNNE</t>
   </si>
   <si>
-    <t>MBRA340T3G</t>
-  </si>
-  <si>
-    <t>Diode</t>
+    <t>SSA34HE3_A_I</t>
+  </si>
+  <si>
+    <t>Schottky Diode</t>
   </si>
   <si>
     <t>D1</t>
   </si>
   <si>
-    <t>DIOM5226X220N</t>
+    <t>DIONM5127X229N</t>
   </si>
   <si>
     <t>DRV8833PWPR</t>
@@ -437,7 +437,7 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{6CCABC8B-7800-4CA1-9D47-B37511B91CFF}"/>
+    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{B7DB2B9C-8090-41CF-BED1-C3885D1E9E55}"/>
   </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -746,12 +746,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB8CE123-5274-46D9-BAA8-2BCC1D5A76C3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA2AADC2-F96C-4C99-BBD0-1A967294DE87}">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>

</xml_diff>

<commit_message>
Replaced backordered part with equivalent.
</commit_message>
<xml_diff>
--- a/Car_Circuitry/Car_Circuitry_BOM.xlsx
+++ b/Car_Circuitry/Car_Circuitry_BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Oasis\Documents\School\Assignments\Undergraduate Year 3\Chem-E Car Team\McMaster_Chem-E_Car_23-24\Car_Circuitry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B370160B-C190-453C-9D6C-E00CA3122208}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA455625-F9AD-49FE-A7F4-C7D5FA7D241B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13620" xr2:uid="{BFB9A709-E0C0-42D2-9C81-D0328AE637B6}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13620" xr2:uid="{7C4C1D7A-DC8F-4684-AA7B-9C3498B008D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Car_Circuitry_BOM" sheetId="1" r:id="rId1"/>
@@ -59,16 +59,16 @@
     <t>Quantity</t>
   </si>
   <si>
-    <t>2601-3102</t>
-  </si>
-  <si>
-    <t>WAGO Terminal Block</t>
+    <t>2604-3102</t>
+  </si>
+  <si>
+    <t>Connector</t>
   </si>
   <si>
     <t>BAT_IN</t>
   </si>
   <si>
-    <t>26013102</t>
+    <t>26043102</t>
   </si>
   <si>
     <t>MP3213DH-LF-P</t>
@@ -379,7 +379,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -437,7 +437,7 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{B7DB2B9C-8090-41CF-BED1-C3885D1E9E55}"/>
+    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{13495767-D579-47BC-AAED-6BB64B3CEC57}"/>
   </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -461,39 +461,39 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="0E2841"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="E8E8E8"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="156082"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="E97132"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="196B24"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="0F9ED5"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="A02B93"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="4EA72E"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="467886"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="96607D"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -545,7 +545,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -656,13 +656,6 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
@@ -671,6 +664,13 @@
           <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -735,30 +735,50 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
+  <a:objectDefaults>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA2AADC2-F96C-4C99-BBD0-1A967294DE87}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42D87CA4-DF68-481F-BB73-0AEC5228FBA2}">
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.81640625" customWidth="1"/>
+    <col min="6" max="6" width="7.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.35">
@@ -1323,6 +1343,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added assembly drawing to PCB
</commit_message>
<xml_diff>
--- a/Car_Circuitry/Car_Circuitry_BOM.xlsx
+++ b/Car_Circuitry/Car_Circuitry_BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Oasis\Documents\School\Assignments\Undergraduate Year 3\Chem-E Car Team\McMaster_Chem-E_Car_23-24\Car_Circuitry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA455625-F9AD-49FE-A7F4-C7D5FA7D241B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3519C40-5C62-4D9C-BA8E-67282E85E024}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13620" xr2:uid="{7C4C1D7A-DC8F-4684-AA7B-9C3498B008D7}"/>
   </bookViews>
@@ -329,46 +329,46 @@
     <t>ERJ-6DSFR18V</t>
   </si>
   <si>
+    <t>R6, R9</t>
+  </si>
+  <si>
+    <t>4.7 kΩ</t>
+  </si>
+  <si>
+    <t>R10</t>
+  </si>
+  <si>
+    <t>RESAD1530W60L610D230</t>
+  </si>
+  <si>
+    <t>CF1_4C472J</t>
+  </si>
+  <si>
+    <t>100 kΩ</t>
+  </si>
+  <si>
+    <t>R11</t>
+  </si>
+  <si>
+    <t>ERJ8ENF1000V</t>
+  </si>
+  <si>
+    <t>ERJ-8ENF1003V</t>
+  </si>
+  <si>
+    <t>732 kΩ</t>
+  </si>
+  <si>
+    <t>R12</t>
+  </si>
+  <si>
+    <t>ERJ-8ENF7323V</t>
+  </si>
+  <si>
     <t>330 mΩ</t>
   </si>
   <si>
-    <t>R6, R9</t>
-  </si>
-  <si>
     <t>ERJ-6DQFR33V</t>
-  </si>
-  <si>
-    <t>4.7 kΩ</t>
-  </si>
-  <si>
-    <t>R10</t>
-  </si>
-  <si>
-    <t>RESAD1530W60L610D230</t>
-  </si>
-  <si>
-    <t>CF1_4C472J</t>
-  </si>
-  <si>
-    <t>100 kΩ</t>
-  </si>
-  <si>
-    <t>R11</t>
-  </si>
-  <si>
-    <t>ERJ8ENF1000V</t>
-  </si>
-  <si>
-    <t>ERJ-8ENF1003V</t>
-  </si>
-  <si>
-    <t>732 kΩ</t>
-  </si>
-  <si>
-    <t>R12</t>
-  </si>
-  <si>
-    <t>ERJ-8ENF7323V</t>
   </si>
 </sst>
 </file>
@@ -769,7 +769,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42D87CA4-DF68-481F-BB73-0AEC5228FBA2}">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1263,19 +1265,19 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
-        <v>96</v>
+        <v>108</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>77</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>94</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>98</v>
+        <v>109</v>
       </c>
       <c r="F25" s="1">
         <v>2</v>
@@ -1283,19 +1285,19 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>77</v>
       </c>
       <c r="C26" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E26" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>102</v>
       </c>
       <c r="F26" s="1">
         <v>1</v>
@@ -1303,19 +1305,19 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>77</v>
       </c>
       <c r="C27" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E27" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>106</v>
       </c>
       <c r="F27" s="1">
         <v>1</v>
@@ -1323,19 +1325,19 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>77</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F28" s="1">
         <v>1</v>

</xml_diff>